<commit_message>
detector with equalize hist
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385" tabRatio="646" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385" tabRatio="646" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bibliotecas" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="80">
   <si>
     <t>Designação</t>
   </si>
@@ -707,6 +707,12 @@
   </si>
   <si>
     <t>LBPH</t>
+  </si>
+  <si>
+    <t>Img Treino</t>
+  </si>
+  <si>
+    <t>Img Teste</t>
   </si>
 </sst>
 </file>
@@ -5025,10 +5031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5039,9 +5045,10 @@
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5063,8 +5070,14 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -5086,8 +5099,14 @@
       <c r="G2">
         <v>20</v>
       </c>
+      <c r="H2">
+        <v>944</v>
+      </c>
+      <c r="I2">
+        <v>236</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -5109,8 +5128,14 @@
       <c r="G3">
         <v>20</v>
       </c>
+      <c r="H3">
+        <v>942</v>
+      </c>
+      <c r="I3">
+        <v>236</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5132,52 +5157,58 @@
       <c r="G4">
         <v>20</v>
       </c>
+      <c r="H4">
+        <v>944</v>
+      </c>
+      <c r="I4">
+        <v>236</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
     </row>
@@ -5208,7 +5239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
@@ -5223,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>